<commit_message>
remove empty worksheets from plants.xlsx
</commit_message>
<xml_diff>
--- a/r4babs2/week-2/data-raw/plant.xlsx
+++ b/r4babs2/week-2/data-raw/plant.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\web\17C - 2018\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\er13\OneDrive - University of York\Desktop\Desktop\undergrad-teaching-york\R4BABS\r4babs2\week-2\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_42148086757A0B0E4F0FCF8CEA85F10AB49FDA12" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6115E89A-4FE1-4879-97BC-63EE31E92163}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="plant" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="plant" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -833,22 +831,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1271,28 +1257,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ 3mmaRand/R4BABS@1315899d5e799e40e68f3bf593269619a66e7b39 🚀
</commit_message>
<xml_diff>
--- a/r4babs2/week-2/data-raw/plant.xlsx
+++ b/r4babs2/week-2/data-raw/plant.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\web\17C - 2018\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\er13\OneDrive - University of York\Desktop\Desktop\undergrad-teaching-york\R4BABS\r4babs2\week-2\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_42148086757A0B0E4F0FCF8CEA85F10AB49FDA12" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6115E89A-4FE1-4879-97BC-63EE31E92163}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="plant" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="plant" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -833,22 +831,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1271,28 +1257,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>